<commit_message>
Add ABW and AGW experimental data. FHY is undermass, need to add mass as a parameter to search for.
</commit_message>
<xml_diff>
--- a/Sorption Experiments/RaAGW_7_7_2017/RaAGW Equilibrated Data.xlsx
+++ b/Sorption Experiments/RaAGW_7_7_2017/RaAGW Equilibrated Data.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Dropbox (Personal)\work\MIT Graduate Work\Research\RadiumSorption\Sorption Experiments\RaAGW_7_7_2017\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Equilibrated Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -70,8 +75,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +139,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -180,7 +193,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -212,9 +225,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -246,6 +260,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -421,14 +436,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,169 +453,169 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>40.73416666666667</v>
+        <v>40.454047619047607</v>
       </c>
       <c r="C2">
-        <v>0.519360625</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>0.51896763945578228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>38.31666666666666</v>
+        <v>38.326428571428558</v>
       </c>
       <c r="C3">
-        <v>0.5038641666666667</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>0.50536133673469386</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>19.97</v>
+        <v>19.988571428571429</v>
       </c>
       <c r="C4">
-        <v>0.3644525</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>0.36464865306122451</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>38.515</v>
+        <v>37.770238095238092</v>
       </c>
       <c r="C5">
-        <v>0.508398</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>0.5023441666666667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>38.90333333333334</v>
+        <v>38.499523809523808</v>
       </c>
       <c r="C6">
-        <v>0.5096336666666668</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>0.50709372789115648</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>28.66</v>
+        <v>28.39595238095238</v>
       </c>
       <c r="C7">
-        <v>0.437065</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>0.43526938435374152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8">
-        <v>28.7975</v>
+        <v>28.653571428571428</v>
       </c>
       <c r="C8">
-        <v>0.437722</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>0.43676229591836752</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>28.37416666666667</v>
+        <v>28.26428571428572</v>
       </c>
       <c r="C9">
-        <v>0.4341247500000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>0.43405867346938781</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B10">
-        <v>40.28</v>
+        <v>39.940714285714293</v>
       </c>
       <c r="C10">
-        <v>0.517598</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>0.51580579591836739</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11">
-        <v>32.06416666666667</v>
+        <v>31.722380952380949</v>
       </c>
       <c r="C11">
-        <v>0.4633272083333333</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>0.45952134693877539</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12">
-        <v>32.86833333333333</v>
+        <v>32.367142857142859</v>
       </c>
       <c r="C12">
-        <v>0.4683737499999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>0.46562446938775509</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13">
-        <v>32.57</v>
+        <v>32.304285714285712</v>
       </c>
       <c r="C13">
-        <v>0.465751</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>0.4637972448979592</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B14">
-        <v>35.56416666666667</v>
+        <v>35.265000000000001</v>
       </c>
       <c r="C14">
-        <v>0.4872290833333333</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>0.48464185714285718</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B15">
-        <v>35.98833333333334</v>
+        <v>35.556904761904768</v>
       </c>
       <c r="C15">
-        <v>0.4894413333333334</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>0.48712959523809529</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B16">
-        <v>36.3</v>
+        <v>35.808809523809529</v>
       </c>
       <c r="C16">
-        <v>0.491865</v>
+        <v>0.48853447278911571</v>
       </c>
     </row>
   </sheetData>

</xml_diff>